<commit_message>
Calculos de sueldo... echo
</commit_message>
<xml_diff>
--- a/EJERCICIO 01 - 25-08-2023.xlsx
+++ b/EJERCICIO 01 - 25-08-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlexRD\Laboratorio\Clase4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D0A75E-D21D-46C5-8608-303EE044FF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8E6EA2-0E46-47E6-B491-FCB398D0ADB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HOJA DE DATOS" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
   <si>
     <t>LEGAJO</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>Sueldo en Pesos</t>
+  </si>
+  <si>
+    <t>Punto Nº 1</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
   </si>
 </sst>
 </file>
@@ -262,7 +271,7 @@
     <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,8 +366,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,8 +413,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -636,13 +672,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -708,9 +759,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -757,6 +805,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -765,31 +820,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
       <fill>
@@ -831,6 +861,32 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1511,6 +1567,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla_empleados" displayName="Tabla_empleados" ref="A2:J22" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A2:J22" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Santa Fe"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="LEGAJO" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NOMBRE" dataDxfId="7"/>
@@ -1519,11 +1582,15 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="PROVINCIA" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="CARGO"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="AÑOS DE TRABAJO" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Edad del empleado" dataDxfId="0">
-      <calculatedColumnFormula>N3735</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Edad del empleado" dataDxfId="2">
+      <calculatedColumnFormula>YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Sueldo en Pesos" dataDxfId="2" dataCellStyle="Moneda"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Sueldo En Dolares" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Sueldo en Pesos" dataDxfId="1" dataCellStyle="Moneda">
+      <calculatedColumnFormula>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Sueldo En Dolares" dataDxfId="0">
+      <calculatedColumnFormula>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1792,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFC24"/>
+  <dimension ref="A1:XFB24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,23 +1870,24 @@
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
-    <col min="12" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14 16383:16383" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14 16382:16382" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="G1" s="3"/>
-      <c r="XFC1">
+      <c r="XFB1">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14 16383:16383" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14 16382:16382" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1841,24 +1909,24 @@
       <c r="G2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="34">
+      <c r="L2" s="33">
         <f ca="1">TODAY()</f>
         <v>45189</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1880,18 +1948,23 @@
       <c r="G3" s="22">
         <v>5</v>
       </c>
-      <c r="H3" s="27">
-        <f t="shared" ref="H3:H22" si="0">N3735</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="24"/>
-      <c r="N3" s="35">
+      <c r="H3" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>25</v>
+      </c>
+      <c r="I3" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>3000000</v>
+      </c>
+      <c r="J3" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>4081.6326530612246</v>
+      </c>
+      <c r="N3" s="34">
         <v>735</v>
       </c>
     </row>
-    <row r="4" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1913,21 +1986,26 @@
       <c r="G4" s="23">
         <v>23</v>
       </c>
-      <c r="H4" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="28" t="s">
+      <c r="H4" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>69</v>
+      </c>
+      <c r="I4" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J4" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+      <c r="L4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1949,21 +2027,26 @@
       <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="26" t="s">
+      <c r="H5" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>60</v>
+      </c>
+      <c r="I5" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J5" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+      <c r="L5" s="25" t="s">
         <v>34</v>
       </c>
       <c r="M5" s="13">
         <v>650000</v>
       </c>
     </row>
-    <row r="6" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1985,21 +2068,26 @@
       <c r="G6" s="23">
         <v>9</v>
       </c>
-      <c r="H6" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="26" t="s">
+      <c r="H6" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>33</v>
+      </c>
+      <c r="I6" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J6" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+      <c r="L6" s="25" t="s">
         <v>35</v>
       </c>
       <c r="M6" s="13">
         <v>1200000</v>
       </c>
     </row>
-    <row r="7" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2021,21 +2109,26 @@
       <c r="G7" s="23">
         <v>7</v>
       </c>
-      <c r="H7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="26" t="s">
+      <c r="H7" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>38</v>
+      </c>
+      <c r="I7" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J7" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+      <c r="L7" s="25" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="13">
         <v>3000000</v>
       </c>
     </row>
-    <row r="8" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2057,15 +2150,20 @@
       <c r="G8" s="23">
         <v>5</v>
       </c>
-      <c r="H8" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="24"/>
-    </row>
-    <row r="9" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>50</v>
+      </c>
+      <c r="I8" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J8" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2087,15 +2185,20 @@
       <c r="G9" s="23">
         <v>8</v>
       </c>
-      <c r="H9" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="24"/>
-    </row>
-    <row r="10" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>28</v>
+      </c>
+      <c r="I9" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J9" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2117,15 +2220,20 @@
       <c r="G10" s="23">
         <v>12</v>
       </c>
-      <c r="H10" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="24"/>
-    </row>
-    <row r="11" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>27</v>
+      </c>
+      <c r="I10" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J10" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2147,15 +2255,20 @@
       <c r="G11" s="23">
         <v>10</v>
       </c>
-      <c r="H11" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="24"/>
-    </row>
-    <row r="12" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>41</v>
+      </c>
+      <c r="I11" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>650000</v>
+      </c>
+      <c r="J11" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>884.35374149659867</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2177,15 +2290,20 @@
       <c r="G12" s="23">
         <v>2</v>
       </c>
-      <c r="H12" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="24"/>
-    </row>
-    <row r="13" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>37</v>
+      </c>
+      <c r="I12" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>650000</v>
+      </c>
+      <c r="J12" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>884.35374149659867</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2207,15 +2325,20 @@
       <c r="G13" s="23">
         <v>1</v>
       </c>
-      <c r="H13" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>30</v>
+      </c>
+      <c r="I13" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>650000</v>
+      </c>
+      <c r="J13" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>884.35374149659867</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2237,15 +2360,20 @@
       <c r="G14" s="23">
         <v>11</v>
       </c>
-      <c r="H14" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="24"/>
-    </row>
-    <row r="15" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>53</v>
+      </c>
+      <c r="I14" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J14" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2267,15 +2395,20 @@
       <c r="G15" s="23">
         <v>2</v>
       </c>
-      <c r="H15" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="24"/>
-    </row>
-    <row r="16" spans="1:14 16383:16383" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>34</v>
+      </c>
+      <c r="I15" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J15" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2297,15 +2430,20 @@
       <c r="G16" s="23">
         <v>3</v>
       </c>
-      <c r="H16" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>33</v>
+      </c>
+      <c r="I16" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>650000</v>
+      </c>
+      <c r="J16" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>884.35374149659867</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2327,15 +2465,20 @@
       <c r="G17" s="23">
         <v>5</v>
       </c>
-      <c r="H17" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="24"/>
-    </row>
-    <row r="18" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>23</v>
+      </c>
+      <c r="I17" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>650000</v>
+      </c>
+      <c r="J17" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>884.35374149659867</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2357,15 +2500,20 @@
       <c r="G18" s="23">
         <v>5</v>
       </c>
-      <c r="H18" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="29"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="24"/>
-    </row>
-    <row r="19" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>28</v>
+      </c>
+      <c r="I18" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>3000000</v>
+      </c>
+      <c r="J18" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>4081.6326530612246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2387,15 +2535,20 @@
       <c r="G19" s="23">
         <v>25</v>
       </c>
-      <c r="H19" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>44</v>
+      </c>
+      <c r="I19" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J19" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2417,15 +2570,20 @@
       <c r="G20" s="23">
         <v>6</v>
       </c>
-      <c r="H20" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="24"/>
-    </row>
-    <row r="21" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>41</v>
+      </c>
+      <c r="I20" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>650000</v>
+      </c>
+      <c r="J20" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>884.35374149659867</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2447,15 +2605,20 @@
       <c r="G21" s="23">
         <v>9</v>
       </c>
-      <c r="H21" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="24"/>
-    </row>
-    <row r="22" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>24</v>
+      </c>
+      <c r="I21" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>650000</v>
+      </c>
+      <c r="J21" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>884.35374149659867</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2477,16 +2640,21 @@
       <c r="G22" s="23">
         <v>2</v>
       </c>
-      <c r="H22" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="24"/>
-    </row>
-    <row r="23" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H22" s="26">
+        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <v>49</v>
+      </c>
+      <c r="I22" s="28">
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
+        <v>1200000</v>
+      </c>
+      <c r="J22" s="29">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2498,20 +2666,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:F19"/>
+  <dimension ref="A2:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>39</v>
       </c>
@@ -2519,7 +2688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>41</v>
       </c>
@@ -2533,37 +2702,46 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="D4" s="25" t="s">
+      <c r="B4" s="30"/>
+      <c r="D4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="E4" s="18">
+        <f>COUNTIF(Tabla_empleados[PROVINCIA],"Cordoba")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="D5" s="25" t="s">
+      <c r="B5" s="30"/>
+      <c r="D5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="E5" s="18">
+        <f>COUNTIF(Tabla_empleados[PROVINCIA],"Santa Fe")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="D6" s="25" t="s">
+      <c r="B6" s="30"/>
+      <c r="D6" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="18">
+        <f>COUNTIF(Tabla_empleados[PROVINCIA],"Buenos Aires")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
@@ -2571,7 +2749,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>43</v>
       </c>
@@ -2580,47 +2758,69 @@
       </c>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:6" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="18"/>
     </row>
-    <row r="13" spans="1:6" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="18"/>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
-    </row>
-    <row r="14" spans="1:6" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="H13" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="18"/>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-    </row>
-    <row r="15" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="32" t="s">
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
+      <c r="H14" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="H15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I17" s="44"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>47</v>
       </c>
@@ -2634,11 +2834,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Punto uno y dos echos
</commit_message>
<xml_diff>
--- a/EJERCICIO 01 - 25-08-2023.xlsx
+++ b/EJERCICIO 01 - 25-08-2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlexRD\Laboratorio\Clase4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Estudios Superiores\ISNPT\Laboratorio\Excel\Clase_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8E6EA2-0E46-47E6-B491-FCB398D0ADB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047FDC98-7713-4A68-8F24-C9FBBB0D12CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="60" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HOJA DE DATOS" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
   <si>
     <t>LEGAJO</t>
   </si>
@@ -259,17 +259,36 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Punto Nº 2</t>
+  </si>
+  <si>
+    <t>Inversion en Pesos</t>
+  </si>
+  <si>
+    <t>Inversion en Dolares</t>
+  </si>
+  <si>
+    <t>Punto Nº 3</t>
+  </si>
+  <si>
+    <t>Max Recaudado en Pesos</t>
+  </si>
+  <si>
+    <t>Max Recaudado en Dolares</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -368,27 +387,25 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,14 +430,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -673,16 +684,42 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="hair">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="hair">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="hair">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="56"/>
+      </left>
+      <right style="medium">
+        <color indexed="56"/>
+      </right>
+      <top style="medium">
+        <color indexed="56"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -693,7 +730,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -806,13 +843,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="16" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
@@ -821,7 +871,22 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -846,22 +911,7 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1567,13 +1617,6 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla_empleados" displayName="Tabla_empleados" ref="A2:J22" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A2:J22" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Santa Fe"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="LEGAJO" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NOMBRE" dataDxfId="7"/>
@@ -1585,10 +1628,10 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Edad del empleado" dataDxfId="2">
       <calculatedColumnFormula>YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Sueldo en Pesos" dataDxfId="1" dataCellStyle="Moneda">
-      <calculatedColumnFormula>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Sueldo en Pesos" dataDxfId="0" dataCellStyle="Moneda">
+      <calculatedColumnFormula>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Sueldo En Dolares" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Sueldo En Dolares" dataDxfId="1">
       <calculatedColumnFormula>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1861,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="A2:J2"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,13 +1963,13 @@
       </c>
       <c r="L2" s="33">
         <f ca="1">TODAY()</f>
-        <v>45189</v>
+        <v>45192</v>
       </c>
       <c r="N2" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1964,7 +2007,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="4" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1991,12 +2034,12 @@
         <v>69</v>
       </c>
       <c r="I4" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J4" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
+        <v>1632.6544217687074</v>
       </c>
       <c r="L4" s="27" t="s">
         <v>37</v>
@@ -2005,7 +2048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2032,12 +2075,12 @@
         <v>60</v>
       </c>
       <c r="I5" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J5" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
+        <v>1632.6544217687074</v>
       </c>
       <c r="L5" s="25" t="s">
         <v>34</v>
@@ -2046,7 +2089,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="6" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2073,12 +2116,12 @@
         <v>33</v>
       </c>
       <c r="I6" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J6" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
+        <v>1632.6544217687074</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>35</v>
@@ -2114,12 +2157,12 @@
         <v>38</v>
       </c>
       <c r="I7" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J7" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
+        <v>1632.6544217687074</v>
       </c>
       <c r="L7" s="25" t="s">
         <v>36</v>
@@ -2155,12 +2198,12 @@
         <v>50</v>
       </c>
       <c r="I8" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J8" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
+        <v>1632.6544217687074</v>
       </c>
     </row>
     <row r="9" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2190,12 +2233,12 @@
         <v>28</v>
       </c>
       <c r="I9" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J9" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
+        <v>1632.6544217687074</v>
       </c>
     </row>
     <row r="10" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2225,15 +2268,15 @@
         <v>27</v>
       </c>
       <c r="I10" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J10" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1632.6544217687074</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2260,15 +2303,15 @@
         <v>41</v>
       </c>
       <c r="I11" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>650000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>650001</v>
       </c>
       <c r="J11" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35374149659867</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>884.35510204081629</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2295,15 +2338,15 @@
         <v>37</v>
       </c>
       <c r="I12" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>650000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>650001</v>
       </c>
       <c r="J12" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35374149659867</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>884.35510204081629</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2330,15 +2373,15 @@
         <v>30</v>
       </c>
       <c r="I13" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>650000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>650001</v>
       </c>
       <c r="J13" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35374149659867</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>884.35510204081629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2365,15 +2408,15 @@
         <v>53</v>
       </c>
       <c r="I14" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J14" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1632.6544217687074</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2400,15 +2443,15 @@
         <v>34</v>
       </c>
       <c r="I15" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J15" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14 16382:16382" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1632.6544217687074</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2435,15 +2478,15 @@
         <v>33</v>
       </c>
       <c r="I16" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>650000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>650001</v>
       </c>
       <c r="J16" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35374149659867</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>884.35510204081629</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2470,15 +2513,15 @@
         <v>23</v>
       </c>
       <c r="I17" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>650000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>650001</v>
       </c>
       <c r="J17" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35374149659867</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>884.35510204081629</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2513,7 +2556,7 @@
         <v>4081.6326530612246</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2540,15 +2583,15 @@
         <v>44</v>
       </c>
       <c r="I19" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J19" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1632.6544217687074</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2575,15 +2618,15 @@
         <v>41</v>
       </c>
       <c r="I20" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>650000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>650001</v>
       </c>
       <c r="J20" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35374149659867</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>884.35510204081629</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2610,15 +2653,15 @@
         <v>24</v>
       </c>
       <c r="I21" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>650000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>650001</v>
       </c>
       <c r="J21" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35374149659867</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="24.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>884.35510204081629</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2645,12 +2688,12 @@
         <v>49</v>
       </c>
       <c r="I22" s="28">
-        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)</f>
-        <v>1200000</v>
+        <f>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</f>
+        <v>1200001</v>
       </c>
       <c r="J22" s="29">
         <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6530612244899</v>
+        <v>1632.6544217687074</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2666,10 +2709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:J19"/>
+  <dimension ref="A2:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2677,10 +2720,13 @@
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>39</v>
       </c>
@@ -2688,7 +2734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>41</v>
       </c>
@@ -2702,7 +2748,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>36</v>
       </c>
@@ -2715,7 +2761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>35</v>
       </c>
@@ -2728,7 +2774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>34</v>
       </c>
@@ -2741,7 +2787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
@@ -2749,7 +2795,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>43</v>
       </c>
@@ -2758,13 +2804,13 @@
       </c>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="18"/>
     </row>
-    <row r="13" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
@@ -2774,11 +2820,14 @@
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="43"/>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="46" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L13" s="46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>33</v>
       </c>
@@ -2788,39 +2837,69 @@
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="40"/>
-      <c r="H14" s="45" t="s">
+      <c r="H14" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="46" t="s">
+      <c r="I14" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="46" t="s">
+      <c r="J14" s="47" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L14" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="O14" s="50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="31" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="38"/>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="49">
+        <f>COUNTIFS(Tabla_empleados[CARGO],resumen!I15,Tabla_empleados[PROVINCIA],resumen!H15)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="51">
+        <f>SUMIFS(Tabla_empleados[Sueldo en Pesos],Tabla_empleados[CARGO],resumen!M15,Tabla_empleados[PROVINCIA],resumen!L15)</f>
+        <v>3000000</v>
+      </c>
+      <c r="O15" s="51">
+        <f>SUMIFS(Tabla_empleados[Sueldo En Dolares],Tabla_empleados[CARGO],resumen!M15,Tabla_empleados[PROVINCIA],resumen!L15)</f>
+        <v>4081.6326530612246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="44"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>47</v>
       </c>
@@ -2833,12 +2912,30 @@
       <c r="D18" s="21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36"/>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
       <c r="D19" s="36"/>
+      <c r="H19" s="53" t="str">
+        <f>_xlfn.XLOOKUP(resumen!I19,Tabla_empleados[Sueldo en Pesos],Tabla_empleados[PROVINCIA])&amp; "," &amp; _xlfn.XLOOKUP(resumen!I19,Tabla_empleados[Sueldo en Pesos],Tabla_empleados[PROVINCIA])</f>
+        <v>Cordoba,Cordoba</v>
+      </c>
+      <c r="I19" s="52">
+        <f>MAX(Tabla_empleados[Sueldo en Pesos])</f>
+        <v>3000000</v>
+      </c>
+      <c r="J19" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Corregir punto 3,9 entre otros
</commit_message>
<xml_diff>
--- a/EJERCICIO 01 - 25-08-2023.xlsx
+++ b/EJERCICIO 01 - 25-08-2023.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Estudios Superiores\ISNPT\Laboratorio\Excel\Clase_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irma\Desktop\Clase_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047FDC98-7713-4A68-8F24-C9FBBB0D12CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="60" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="60" windowWidth="15380" windowHeight="7880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HOJA DE DATOS" sheetId="1" r:id="rId1"/>
     <sheet name="resumen" sheetId="2" r:id="rId2"/>
     <sheet name="Grafico" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Alex</author>
   </authors>
   <commentList>
-    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
   <si>
     <t>LEGAJO</t>
   </si>
@@ -277,18 +276,30 @@
   </si>
   <si>
     <t>Max Recaudado en Dolares</t>
+  </si>
+  <si>
+    <t>Preguntar a que se refiere por empresa</t>
+  </si>
+  <si>
+    <t>Preguntar como sacar el nombre de Bs As</t>
+  </si>
+  <si>
+    <t>Euro hoy</t>
+  </si>
+  <si>
+    <t>Sueldo en Euros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -405,7 +416,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,8 +441,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -724,13 +741,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -822,27 +926,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -861,32 +944,81 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="16" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -911,7 +1043,22 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1076,7 +1223,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1297,6 +1444,2803 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Punto 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resumen!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Abogado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>resumen!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ocupación</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>resumen!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6456-48A0-B27D-4DBF7589ABFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resumen!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gerente</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>resumen!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ocupación</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>resumen!$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6456-48A0-B27D-4DBF7589ABFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resumen!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Administrativo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>resumen!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ocupación</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>resumen!$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6456-48A0-B27D-4DBF7589ABFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="885026992"/>
+        <c:axId val="885027408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="885026992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885027408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="885027408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885026992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Cantidad de Empleados</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resumen!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cantidad Empleados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-CB6C-4386-AF4D-D9526505FDB5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CB6C-4386-AF4D-D9526505FDB5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-CB6C-4386-AF4D-D9526505FDB5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>resumen!$D$4:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Cordoba</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Santa Fe</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Buenos Aires</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>resumen!$E$4:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-CB6C-4386-AF4D-D9526505FDB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Suma de Sueldo en Pesos por CARGO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>Abogado</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Administrativo</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Gerente</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>6000000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>4550007</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>13200011</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9379-4A1F-B8D4-A264132132DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="885781152"/>
+        <c:axId val="885773664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="885781152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885773664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="885773664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885781152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="266">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1604,35 +4548,137 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41275</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>41275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tabla_sueldos" displayName="tabla_sueldos" ref="L4:M7" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="L4:M7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabla_sueldos" displayName="tabla_sueldos" ref="M4:N7" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="M4:N7"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CARGO" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUELDO" dataDxfId="10" dataCellStyle="Moneda"/>
+    <tableColumn id="1" name="CARGO" dataDxfId="12"/>
+    <tableColumn id="2" name="SUELDO" dataDxfId="11" dataCellStyle="Moneda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla_empleados" displayName="Tabla_empleados" ref="A2:J22" totalsRowShown="0" headerRowDxfId="9">
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="LEGAJO" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NOMBRE" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="FECHA DE NAC." dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="LOCALIDAD" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="PROVINCIA" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="CARGO"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="AÑOS DE TRABAJO" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Edad del empleado" dataDxfId="2">
-      <calculatedColumnFormula>YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla_empleados" displayName="Tabla_empleados" ref="A2:K22" totalsRowShown="0" headerRowDxfId="10">
+  <tableColumns count="11">
+    <tableColumn id="1" name="LEGAJO" dataDxfId="9"/>
+    <tableColumn id="2" name="NOMBRE" dataDxfId="8"/>
+    <tableColumn id="3" name="FECHA DE NAC." dataDxfId="7"/>
+    <tableColumn id="4" name="LOCALIDAD" dataDxfId="6"/>
+    <tableColumn id="5" name="PROVINCIA" dataDxfId="5"/>
+    <tableColumn id="6" name="CARGO"/>
+    <tableColumn id="7" name="AÑOS DE TRABAJO" dataDxfId="4"/>
+    <tableColumn id="8" name="Edad del empleado" dataDxfId="3">
+      <calculatedColumnFormula>YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Sueldo en Pesos" dataDxfId="0" dataCellStyle="Moneda">
+    <tableColumn id="9" name="Sueldo en Pesos" dataDxfId="2" dataCellStyle="Moneda">
       <calculatedColumnFormula>VLOOKUP(Tabla_empleados[[#This Row],[CARGO]],tabla_sueldos[],2,FALSE)+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Sueldo En Dolares" dataDxfId="1">
-      <calculatedColumnFormula>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</calculatedColumnFormula>
+    <tableColumn id="10" name="Sueldo En Dolares" dataDxfId="1">
+      <calculatedColumnFormula>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="Sueldo en Euros" dataDxfId="0">
+      <calculatedColumnFormula>I3/P$3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1901,36 +4947,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFB24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFC24"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" customWidth="1"/>
-    <col min="11" max="12" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" customWidth="1"/>
+    <col min="8" max="8" width="20.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
+    <col min="10" max="10" width="19.81640625" customWidth="1"/>
+    <col min="11" max="11" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.08984375" customWidth="1"/>
+    <col min="13" max="13" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14 16382:16382" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16 16383:16383" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="G1" s="3"/>
-      <c r="XFB1">
+      <c r="XFC1">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14 16382:16382" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16 16383:16383" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1961,15 +5010,22 @@
       <c r="J2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="33">
+      <c r="K2" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="58"/>
+      <c r="M2" s="33">
         <f ca="1">TODAY()</f>
-        <v>45192</v>
-      </c>
-      <c r="N2" s="32" t="s">
+        <v>45195</v>
+      </c>
+      <c r="O2" s="32" t="s">
         <v>55</v>
       </c>
+      <c r="P2" s="32" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="3" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1992,7 +5048,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>25</v>
       </c>
       <c r="I3" s="28">
@@ -2000,14 +5056,22 @@
         <v>3000000</v>
       </c>
       <c r="J3" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>4081.6326530612246</v>
-      </c>
-      <c r="N3" s="34">
-        <v>735</v>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>4026.8456375838928</v>
+      </c>
+      <c r="K3" s="29">
+        <f t="shared" ref="K3:K22" si="0">I3/P$3</f>
+        <v>4054.0540540540542</v>
+      </c>
+      <c r="L3" s="59"/>
+      <c r="O3" s="34">
+        <v>745</v>
+      </c>
+      <c r="P3" s="34">
+        <v>740</v>
       </c>
     </row>
-    <row r="4" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2030,7 +5094,7 @@
         <v>23</v>
       </c>
       <c r="H4" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>69</v>
       </c>
       <c r="I4" s="28">
@@ -2038,17 +5102,22 @@
         <v>1200001</v>
       </c>
       <c r="J4" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
-      <c r="L4" s="27" t="s">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K4" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L4" s="59"/>
+      <c r="M4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="N4" s="27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2071,7 +5140,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>60</v>
       </c>
       <c r="I5" s="28">
@@ -2079,17 +5148,22 @@
         <v>1200001</v>
       </c>
       <c r="J5" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
-      <c r="L5" s="25" t="s">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K5" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L5" s="59"/>
+      <c r="M5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="13">
+      <c r="N5" s="13">
         <v>650000</v>
       </c>
     </row>
-    <row r="6" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2112,7 +5186,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>33</v>
       </c>
       <c r="I6" s="28">
@@ -2120,17 +5194,22 @@
         <v>1200001</v>
       </c>
       <c r="J6" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
-      <c r="L6" s="25" t="s">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K6" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L6" s="59"/>
+      <c r="M6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="13">
+      <c r="N6" s="13">
         <v>1200000</v>
       </c>
     </row>
-    <row r="7" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2153,7 +5232,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>38</v>
       </c>
       <c r="I7" s="28">
@@ -2161,17 +5240,22 @@
         <v>1200001</v>
       </c>
       <c r="J7" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
-      <c r="L7" s="25" t="s">
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K7" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L7" s="59"/>
+      <c r="M7" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="13">
+      <c r="N7" s="13">
         <v>3000000</v>
       </c>
     </row>
-    <row r="8" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2194,7 +5278,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>50</v>
       </c>
       <c r="I8" s="28">
@@ -2202,11 +5286,16 @@
         <v>1200001</v>
       </c>
       <c r="J8" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K8" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L8" s="59"/>
     </row>
-    <row r="9" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2229,7 +5318,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>28</v>
       </c>
       <c r="I9" s="28">
@@ -2237,11 +5326,16 @@
         <v>1200001</v>
       </c>
       <c r="J9" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K9" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L9" s="59"/>
     </row>
-    <row r="10" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2264,7 +5358,7 @@
         <v>12</v>
       </c>
       <c r="H10" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>27</v>
       </c>
       <c r="I10" s="28">
@@ -2272,11 +5366,16 @@
         <v>1200001</v>
       </c>
       <c r="J10" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K10" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L10" s="59"/>
     </row>
-    <row r="11" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2299,7 +5398,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>41</v>
       </c>
       <c r="I11" s="28">
@@ -2307,11 +5406,16 @@
         <v>650001</v>
       </c>
       <c r="J11" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35510204081629</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>872.4845637583893</v>
+      </c>
+      <c r="K11" s="29">
+        <f t="shared" si="0"/>
+        <v>878.37972972972977</v>
+      </c>
+      <c r="L11" s="59"/>
     </row>
-    <row r="12" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2334,7 +5438,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>37</v>
       </c>
       <c r="I12" s="28">
@@ -2342,11 +5446,16 @@
         <v>650001</v>
       </c>
       <c r="J12" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35510204081629</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>872.4845637583893</v>
+      </c>
+      <c r="K12" s="29">
+        <f t="shared" si="0"/>
+        <v>878.37972972972977</v>
+      </c>
+      <c r="L12" s="59"/>
     </row>
-    <row r="13" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2369,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>30</v>
       </c>
       <c r="I13" s="28">
@@ -2377,11 +5486,16 @@
         <v>650001</v>
       </c>
       <c r="J13" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35510204081629</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>872.4845637583893</v>
+      </c>
+      <c r="K13" s="29">
+        <f t="shared" si="0"/>
+        <v>878.37972972972977</v>
+      </c>
+      <c r="L13" s="59"/>
     </row>
-    <row r="14" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2404,7 +5518,7 @@
         <v>11</v>
       </c>
       <c r="H14" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>53</v>
       </c>
       <c r="I14" s="28">
@@ -2412,11 +5526,16 @@
         <v>1200001</v>
       </c>
       <c r="J14" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K14" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L14" s="59"/>
     </row>
-    <row r="15" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2439,7 +5558,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>34</v>
       </c>
       <c r="I15" s="28">
@@ -2447,11 +5566,16 @@
         <v>1200001</v>
       </c>
       <c r="J15" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K15" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L15" s="59"/>
     </row>
-    <row r="16" spans="1:14 16382:16382" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16 16383:16383" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2474,7 +5598,7 @@
         <v>3</v>
       </c>
       <c r="H16" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>33</v>
       </c>
       <c r="I16" s="28">
@@ -2482,11 +5606,16 @@
         <v>650001</v>
       </c>
       <c r="J16" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35510204081629</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>872.4845637583893</v>
+      </c>
+      <c r="K16" s="29">
+        <f t="shared" si="0"/>
+        <v>878.37972972972977</v>
+      </c>
+      <c r="L16" s="59"/>
     </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2509,7 +5638,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>23</v>
       </c>
       <c r="I17" s="28">
@@ -2517,11 +5646,16 @@
         <v>650001</v>
       </c>
       <c r="J17" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35510204081629</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>872.4845637583893</v>
+      </c>
+      <c r="K17" s="29">
+        <f t="shared" si="0"/>
+        <v>878.37972972972977</v>
+      </c>
+      <c r="L17" s="59"/>
     </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2544,7 +5678,7 @@
         <v>5</v>
       </c>
       <c r="H18" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>28</v>
       </c>
       <c r="I18" s="28">
@@ -2552,11 +5686,16 @@
         <v>3000000</v>
       </c>
       <c r="J18" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>4081.6326530612246</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>4026.8456375838928</v>
+      </c>
+      <c r="K18" s="29">
+        <f t="shared" si="0"/>
+        <v>4054.0540540540542</v>
+      </c>
+      <c r="L18" s="59"/>
     </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2579,7 +5718,7 @@
         <v>25</v>
       </c>
       <c r="H19" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>44</v>
       </c>
       <c r="I19" s="28">
@@ -2587,11 +5726,16 @@
         <v>1200001</v>
       </c>
       <c r="J19" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K19" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L19" s="59"/>
     </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2614,7 +5758,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>41</v>
       </c>
       <c r="I20" s="28">
@@ -2622,11 +5766,16 @@
         <v>650001</v>
       </c>
       <c r="J20" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35510204081629</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>872.4845637583893</v>
+      </c>
+      <c r="K20" s="29">
+        <f t="shared" si="0"/>
+        <v>878.37972972972977</v>
+      </c>
+      <c r="L20" s="59"/>
     </row>
-    <row r="21" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2649,7 +5798,7 @@
         <v>9</v>
       </c>
       <c r="H21" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>24</v>
       </c>
       <c r="I21" s="28">
@@ -2657,11 +5806,16 @@
         <v>650001</v>
       </c>
       <c r="J21" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>884.35510204081629</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>872.4845637583893</v>
+      </c>
+      <c r="K21" s="29">
+        <f t="shared" si="0"/>
+        <v>878.37972972972977</v>
+      </c>
+      <c r="L21" s="59"/>
     </row>
-    <row r="22" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2684,7 +5838,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="26">
-        <f ca="1">YEAR(L$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
+        <f ca="1">YEAR(M$2)-YEAR(Tabla_empleados[[#This Row],[FECHA DE NAC.]])</f>
         <v>49</v>
       </c>
       <c r="I22" s="28">
@@ -2692,12 +5846,17 @@
         <v>1200001</v>
       </c>
       <c r="J22" s="29">
-        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/N$3</f>
-        <v>1632.6544217687074</v>
-      </c>
+        <f>Tabla_empleados[[#This Row],[Sueldo en Pesos]]/O$3</f>
+        <v>1610.7395973154362</v>
+      </c>
+      <c r="K22" s="29">
+        <f t="shared" si="0"/>
+        <v>1621.622972972973</v>
+      </c>
+      <c r="L22" s="59"/>
     </row>
-    <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2708,25 +5867,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:O19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>39</v>
       </c>
@@ -2734,7 +5893,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>41</v>
       </c>
@@ -2748,46 +5907,61 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="30">
+        <f>COUNTIF(Tabla_empleados[CARGO],resumen!A4)</f>
+        <v>2</v>
+      </c>
       <c r="D4" s="24" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="18">
-        <f>COUNTIF(Tabla_empleados[PROVINCIA],"Cordoba")</f>
+        <f>COUNTIF(Tabla_empleados[PROVINCIA],D4)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="30">
+        <f>COUNTIF(Tabla_empleados[CARGO],resumen!A5)</f>
+        <v>11</v>
+      </c>
       <c r="D5" s="24" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="18">
-        <f>COUNTIF(Tabla_empleados[PROVINCIA],"Santa Fe")</f>
+        <f>COUNTIF(Tabla_empleados[PROVINCIA],D5)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="30">
+        <f>COUNTIF(Tabla_empleados[CARGO],resumen!A6)</f>
+        <v>7</v>
+      </c>
       <c r="D6" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="18">
-        <f>COUNTIF(Tabla_empleados[PROVINCIA],"Buenos Aires")</f>
+        <f>COUNTIF(Tabla_empleados[PROVINCIA],D6)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="54"/>
+    </row>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
@@ -2795,39 +5969,42 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="15">
+        <f>COUNTIF(Tabla_empleados[AÑOS DE TRABAJO],"&gt;5")</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="18"/>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="H13" s="46" t="s">
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="H13" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="46" t="s">
+      <c r="L13" s="39" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="24" t="s">
         <v>33</v>
       </c>
@@ -2835,71 +6012,74 @@
       <c r="D14" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="H14" s="44" t="s">
+      <c r="E14" s="61">
+        <f>MAX('HOJA DE DATOS'!I3:I22)</f>
+        <v>3000000</v>
+      </c>
+      <c r="F14" s="47"/>
+      <c r="H14" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="L14" s="44" t="s">
+      <c r="L14" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="47" t="s">
+      <c r="M14" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="N14" s="50" t="s">
+      <c r="N14" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="O14" s="50" t="s">
+      <c r="O14" s="43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D15" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="H15" s="45" t="s">
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+      <c r="H15" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="49">
+      <c r="J15" s="42">
         <f>COUNTIFS(Tabla_empleados[CARGO],resumen!I15,Tabla_empleados[PROVINCIA],resumen!H15)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="45" t="s">
+      <c r="L15" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="48" t="s">
+      <c r="M15" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="51">
+      <c r="N15" s="44">
         <f>SUMIFS(Tabla_empleados[Sueldo en Pesos],Tabla_empleados[CARGO],resumen!M15,Tabla_empleados[PROVINCIA],resumen!L15)</f>
         <v>3000000</v>
       </c>
-      <c r="O15" s="51">
+      <c r="O15" s="44">
         <f>SUMIFS(Tabla_empleados[Sueldo En Dolares],Tabla_empleados[CARGO],resumen!M15,Tabla_empleados[PROVINCIA],resumen!L15)</f>
-        <v>4081.6326530612246</v>
+        <v>4026.8456375838928</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="46" t="s">
+      <c r="H17" s="39" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="21" t="s">
         <v>47</v>
       </c>
@@ -2912,52 +6092,90 @@
       <c r="D18" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="H18" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="50" t="s">
+      <c r="I18" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="43" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="H19" s="53" t="str">
-        <f>_xlfn.XLOOKUP(resumen!I19,Tabla_empleados[Sueldo en Pesos],Tabla_empleados[PROVINCIA])&amp; "," &amp; _xlfn.XLOOKUP(resumen!I19,Tabla_empleados[Sueldo en Pesos],Tabla_empleados[PROVINCIA])</f>
-        <v>Cordoba,Cordoba</v>
+    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="63">
+        <v>4</v>
+      </c>
+      <c r="B19" s="36" t="str">
+        <f>VLOOKUP(A19,Tabla_empleados[[LEGAJO]:[NOMBRE]],2,FALSE)</f>
+        <v>María</v>
+      </c>
+      <c r="C19" s="36" t="str">
+        <f>VLOOKUP(A19,Tabla_empleados[[LEGAJO]:[CARGO]],6,FALSE)</f>
+        <v>Gerente</v>
+      </c>
+      <c r="D19" s="62">
+        <f>VLOOKUP(resumen!A19,Tabla_empleados[[LEGAJO]:[Sueldo en Pesos]],9,FALSE)</f>
+        <v>1200001</v>
+      </c>
+      <c r="H19" s="51" t="str">
+        <f>INDEX(Tabla_empleados[[PROVINCIA]:[Sueldo en Pesos]],MATCH(I19,Tabla_empleados[Sueldo en Pesos]),1)</f>
+        <v>Cordoba</v>
       </c>
       <c r="I19" s="52">
         <f>MAX(Tabla_empleados[Sueldo en Pesos])</f>
         <v>3000000</v>
       </c>
-      <c r="J19" s="49"/>
+      <c r="J19" s="53">
+        <f>MAX(Tabla_empleados[Sueldo En Dolares])</f>
+        <v>4026.8456375838928</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H20" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="56"/>
+      <c r="J20" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="H20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'HOJA DE DATOS'!$A$3:$A$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>A19</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>